<commit_message>
Update Intervention outcomes and spillover effects.xlsx
Adding sources for measurements in Intervention outcome and spillover effects
</commit_message>
<xml_diff>
--- a/Intervention outcomes and spillover effects/Intervention outcomes and spillover effects.xlsx
+++ b/Intervention outcomes and spillover effects/Intervention outcomes and spillover effects.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Galenos Project/Github preparation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Documents/GitHub/mental-health-ontology/Intervention outcomes and spillover effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="11_D295A90A2C535A10C2167341E065F5EB470CA969" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D96078B-E93F-4DCA-A47E-5FD5CCE42D31}"/>
+  <xr:revisionPtr revIDLastSave="376" documentId="11_D295A90A2C535A10C2167341E065F5EB470CA969" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B97DFB90-111B-45E6-B098-AE1ACF497864}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-15" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$V$98</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="318">
   <si>
     <t>ID</t>
   </si>
@@ -981,6 +984,12 @@
   </si>
   <si>
     <t>PS</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/3616518/</t>
+  </si>
+  <si>
+    <t>https://movementdisorders.onlinelibrary.wiley.com/doi/full/10.1002/mds.22575</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1133,45 +1142,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1196,15 +1182,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1820,11 +1805,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:V98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1840,7 +1826,7 @@
     <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.7265625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.453125" customWidth="1"/>
     <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
@@ -1858,7 +1844,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1888,7 +1874,7 @@
       <c r="K1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1909,7 +1895,7 @@
       <c r="R1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="28" t="s">
         <v>13</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -1918,11 +1904,11 @@
       <c r="U1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -1939,7 +1925,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="L2" s="23"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1959,7 +1945,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>49</v>
       </c>
@@ -1978,7 +1964,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="L3" s="23"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -1998,7 +1984,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>50</v>
       </c>
@@ -2017,7 +2003,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="L4" s="23"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -2037,7 +2023,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>51</v>
       </c>
@@ -2056,7 +2042,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="L5" s="23"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -2076,7 +2062,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>52</v>
       </c>
@@ -2095,7 +2081,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="L6" s="23"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -2115,7 +2101,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
@@ -2134,7 +2120,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="L7" s="23"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -2154,7 +2140,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="12" t="s">
         <v>38</v>
@@ -2174,7 +2160,7 @@
       <c r="K8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="23"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -2194,7 +2180,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="12" t="s">
         <v>40</v>
@@ -2212,7 +2198,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="23"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -2232,7 +2218,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="12" t="s">
         <v>42</v>
@@ -2252,7 +2238,7 @@
       <c r="K10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="23"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -2272,7 +2258,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="12" t="s">
         <v>44</v>
@@ -2292,7 +2278,7 @@
       <c r="K11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="23"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -2312,17 +2298,17 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -2334,7 +2320,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="23"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -2356,13 +2342,13 @@
     </row>
     <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E13" s="9"/>
@@ -2373,8 +2359,10 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="23"/>
+      <c r="K13" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -2394,15 +2382,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E14" s="9"/>
@@ -2412,7 +2400,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="23"/>
+      <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -2432,15 +2420,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="9"/>
@@ -2450,7 +2438,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="23"/>
+      <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
@@ -2472,17 +2460,17 @@
         <v>315</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="6"/>
@@ -2492,7 +2480,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="23"/>
+      <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -2525,14 +2513,14 @@
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="26" t="s">
         <v>291</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="23"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -2554,15 +2542,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="6"/>
@@ -2574,7 +2562,7 @@
       <c r="K18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L18" s="23"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -2596,13 +2584,13 @@
     </row>
     <row r="19" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E19" s="6"/>
@@ -2613,8 +2601,10 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="23"/>
+      <c r="K19" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -2634,15 +2624,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="6"/>
@@ -2652,7 +2642,7 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="23"/>
+      <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -2693,8 +2683,10 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="23"/>
+      <c r="K21" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -2718,25 +2710,25 @@
     </row>
     <row r="22" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="11" t="s">
         <v>294</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="23"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -2758,7 +2750,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
         <v>84</v>
@@ -2778,7 +2770,7 @@
       <c r="K23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L23" s="23"/>
+      <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -2811,14 +2803,16 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="1" t="s">
         <v>295</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="23"/>
+      <c r="K24" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -2840,7 +2834,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>88</v>
@@ -2858,7 +2852,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="23"/>
+      <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -2896,8 +2890,8 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="23"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
@@ -2919,7 +2913,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
         <v>93</v>
@@ -2936,7 +2930,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="23"/>
+      <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -2976,7 +2970,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="23"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -2998,7 +2992,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="1" t="s">
         <v>97</v>
@@ -3016,7 +3010,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="23"/>
+      <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -3056,7 +3050,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="7"/>
-      <c r="L30" s="23"/>
+      <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -3078,7 +3072,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="12" t="s">
         <v>108</v>
@@ -3095,7 +3089,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="23"/>
+      <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -3115,7 +3109,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="12" t="s">
         <v>106</v>
@@ -3133,7 +3127,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="7"/>
-      <c r="L32" s="23"/>
+      <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
@@ -3173,7 +3167,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="23"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
@@ -3197,7 +3191,7 @@
     </row>
     <row r="34" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -3215,7 +3209,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="23"/>
+      <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -3239,7 +3233,7 @@
     </row>
     <row r="35" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -3256,10 +3250,10 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="38" t="s">
+      <c r="K35" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="L35" s="23"/>
+      <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -3281,7 +3275,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="12" t="s">
         <v>114</v>
@@ -3299,7 +3293,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="23"/>
+      <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
@@ -3339,7 +3333,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="23"/>
+      <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
@@ -3381,7 +3375,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="23"/>
+      <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
@@ -3405,25 +3399,25 @@
     </row>
     <row r="39" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="36" t="s">
+      <c r="G39" s="27" t="s">
         <v>306</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="23"/>
+      <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
@@ -3445,25 +3439,25 @@
     </row>
     <row r="40" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="13" t="s">
         <v>123</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="36" t="s">
+      <c r="G40" s="27" t="s">
         <v>305</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="23"/>
+      <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
@@ -3487,25 +3481,25 @@
     </row>
     <row r="41" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="13" t="s">
         <v>123</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="36" t="s">
+      <c r="G41" s="27" t="s">
         <v>307</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="7"/>
-      <c r="L41" s="23"/>
+      <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
@@ -3527,15 +3521,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="6"/>
@@ -3545,7 +3539,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="7"/>
-      <c r="L42" s="23"/>
+      <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
@@ -3565,15 +3559,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E43" s="6"/>
@@ -3583,7 +3577,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="23"/>
+      <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
@@ -3603,15 +3597,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E44" s="6"/>
@@ -3621,7 +3615,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="23"/>
+      <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
@@ -3641,25 +3635,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="24" t="s">
+      <c r="L45" s="19" t="s">
         <v>152</v>
       </c>
       <c r="M45" s="6"/>
@@ -3681,25 +3675,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="23"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="23"/>
+      <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
@@ -3719,25 +3713,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="23"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="23"/>
+      <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
@@ -3757,25 +3751,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E48" s="23"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="23"/>
+      <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
@@ -3795,25 +3789,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E49" s="23"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="23"/>
+      <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
@@ -3833,25 +3827,25 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="24" t="s">
+      <c r="L50" s="19" t="s">
         <v>151</v>
       </c>
       <c r="M50" s="6"/>
@@ -3873,15 +3867,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E51" s="6"/>
@@ -3891,7 +3885,7 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="7"/>
-      <c r="L51" s="24" t="s">
+      <c r="L51" s="19" t="s">
         <v>171</v>
       </c>
       <c r="M51" s="6"/>
@@ -3913,15 +3907,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E52" s="6"/>
@@ -3931,7 +3925,7 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="7"/>
-      <c r="L52" s="23"/>
+      <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
@@ -3951,15 +3945,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6"/>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E53" s="6"/>
@@ -3969,7 +3963,7 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="7"/>
-      <c r="L53" s="23"/>
+      <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
@@ -3989,15 +3983,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E54" s="6"/>
@@ -4007,7 +4001,7 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="23"/>
+      <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
@@ -4027,15 +4021,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E55" s="6"/>
@@ -4045,7 +4039,7 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="23"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
@@ -4065,15 +4059,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E56" s="6"/>
@@ -4085,7 +4079,7 @@
       <c r="K56" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L56" s="23"/>
+      <c r="L56" s="6"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
@@ -4105,15 +4099,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E57" s="6"/>
@@ -4123,7 +4117,7 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="23"/>
+      <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
@@ -4143,15 +4137,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E58" s="6"/>
@@ -4162,7 +4156,7 @@
       <c r="K58" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L58" s="17" t="s">
+      <c r="L58" s="9" t="s">
         <v>174</v>
       </c>
       <c r="M58" s="6"/>
@@ -4184,15 +4178,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E59" s="6"/>
@@ -4202,7 +4196,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="7"/>
-      <c r="L59" s="23"/>
+      <c r="L59" s="6"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
@@ -4222,15 +4216,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E60" s="6"/>
@@ -4242,7 +4236,7 @@
       <c r="K60" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="L60" s="29" t="s">
+      <c r="L60" s="20" t="s">
         <v>183</v>
       </c>
       <c r="M60" s="6"/>
@@ -4264,15 +4258,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E61" s="6"/>
@@ -4284,7 +4278,7 @@
       <c r="K61" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="L61" s="29" t="s">
+      <c r="L61" s="20" t="s">
         <v>184</v>
       </c>
       <c r="M61" s="6"/>
@@ -4308,25 +4302,25 @@
     </row>
     <row r="62" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="36" t="s">
+      <c r="G62" s="27" t="s">
         <v>308</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="23"/>
+      <c r="L62" s="6"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
@@ -4348,25 +4342,25 @@
     </row>
     <row r="63" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
-      <c r="G63" s="36" t="s">
+      <c r="G63" s="27" t="s">
         <v>309</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="7"/>
-      <c r="L63" s="23"/>
+      <c r="L63" s="6"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
@@ -4388,25 +4382,25 @@
     </row>
     <row r="64" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
-      <c r="G64" s="36" t="s">
+      <c r="G64" s="27" t="s">
         <v>310</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="23"/>
+      <c r="L64" s="6"/>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
@@ -4426,15 +4420,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E65" s="6"/>
@@ -4444,7 +4438,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
       <c r="K65" s="7"/>
-      <c r="L65" s="23"/>
+      <c r="L65" s="6"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
@@ -4464,25 +4458,25 @@
     </row>
     <row r="66" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
-      <c r="G66" s="36" t="s">
+      <c r="G66" s="27" t="s">
         <v>311</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="7"/>
-      <c r="L66" s="23"/>
+      <c r="L66" s="6"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
@@ -4502,15 +4496,15 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="1" t="s">
         <v>198</v>
       </c>
       <c r="E67" s="6"/>
@@ -4522,7 +4516,7 @@
       <c r="K67" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L67" s="41" t="s">
+      <c r="L67" s="30" t="s">
         <v>201</v>
       </c>
       <c r="M67" s="6"/>
@@ -4544,25 +4538,25 @@
     </row>
     <row r="68" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="36" t="s">
+      <c r="G68" s="27" t="s">
         <v>312</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
       <c r="K68" s="7"/>
-      <c r="L68" s="23"/>
+      <c r="L68" s="6"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
@@ -4582,9 +4576,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
-      <c r="B69" s="25" t="s">
+      <c r="B69" s="12" t="s">
         <v>204</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -4602,7 +4596,7 @@
       <c r="K69" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L69" s="23"/>
+      <c r="L69" s="6"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
@@ -4622,7 +4616,7 @@
     </row>
     <row r="70" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="12" t="s">
         <v>206</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -4640,7 +4634,7 @@
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
       <c r="K70" s="7"/>
-      <c r="L70" s="23"/>
+      <c r="L70" s="6"/>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
@@ -4662,7 +4656,7 @@
     </row>
     <row r="71" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="12" t="s">
         <v>198</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -4679,10 +4673,10 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
-      <c r="K71" s="16" t="s">
+      <c r="K71" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L71" s="29" t="s">
+      <c r="L71" s="20" t="s">
         <v>215</v>
       </c>
       <c r="M71" s="6"/>
@@ -4704,7 +4698,7 @@
     </row>
     <row r="72" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
-      <c r="B72" s="25" t="s">
+      <c r="B72" s="12" t="s">
         <v>210</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -4722,7 +4716,7 @@
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
       <c r="K72" s="7"/>
-      <c r="L72" s="23"/>
+      <c r="L72" s="6"/>
       <c r="M72" s="6"/>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
@@ -4742,85 +4736,85 @@
         <v>315</v>
       </c>
     </row>
-    <row r="73" spans="1:22" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="23"/>
-      <c r="B73" s="16" t="s">
+    <row r="73" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="6"/>
+      <c r="B73" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="D73" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="16" t="s">
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-      <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-      <c r="P73" s="26">
-        <v>3</v>
-      </c>
-      <c r="Q73" s="16"/>
-      <c r="R73" s="27"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="7"/>
       <c r="S73" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="T73" s="23"/>
-      <c r="U73" s="23"/>
+      <c r="T73" s="6"/>
+      <c r="U73" s="6"/>
       <c r="V73" s="9" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="74" spans="1:22" s="28" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A74" s="23"/>
-      <c r="B74" s="16" t="s">
+    <row r="74" spans="1:22" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="6"/>
+      <c r="B74" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="23"/>
-      <c r="K74" s="16" t="s">
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="L74" s="23"/>
-      <c r="M74" s="23"/>
-      <c r="N74" s="23"/>
-      <c r="O74" s="23"/>
-      <c r="P74" s="26">
-        <v>3</v>
-      </c>
-      <c r="Q74" s="16"/>
-      <c r="R74" s="27"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="7"/>
       <c r="S74" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="T74" s="23"/>
-      <c r="U74" s="23"/>
+      <c r="T74" s="6"/>
+      <c r="U74" s="6"/>
       <c r="V74" s="9" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
-      <c r="B75" s="25" t="s">
+      <c r="B75" s="12" t="s">
         <v>222</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -4836,7 +4830,7 @@
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="7"/>
-      <c r="L75" s="23"/>
+      <c r="L75" s="6"/>
       <c r="M75" s="6"/>
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
@@ -4853,9 +4847,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="12" t="s">
         <v>224</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -4871,7 +4865,7 @@
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
       <c r="K76" s="7"/>
-      <c r="L76" s="23"/>
+      <c r="L76" s="6"/>
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
@@ -4891,9 +4885,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
-      <c r="B77" s="25" t="s">
+      <c r="B77" s="12" t="s">
         <v>228</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -4909,7 +4903,7 @@
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
       <c r="K77" s="7"/>
-      <c r="L77" s="23"/>
+      <c r="L77" s="6"/>
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
@@ -4927,28 +4921,28 @@
         <v>315</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
-      <c r="B78" s="20" t="s">
+      <c r="B78" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-      <c r="K78" s="16"/>
-      <c r="L78" s="23"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
       <c r="P78" s="8">
         <v>3</v>
       </c>
@@ -4964,31 +4958,31 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C79" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17" t="s">
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="16"/>
-      <c r="L79" s="23"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+      <c r="O79" s="9"/>
       <c r="P79" s="8">
         <v>3</v>
       </c>
@@ -5003,30 +4997,30 @@
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="17" t="s">
+    <row r="80" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="23"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+      <c r="O80" s="9"/>
       <c r="P80" s="8">
         <v>3</v>
       </c>
@@ -5041,28 +5035,28 @@
         <v>315</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="17"/>
-      <c r="B81" s="20" t="s">
+    <row r="81" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="9"/>
+      <c r="B81" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="C81" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="16"/>
-      <c r="L81" s="23"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
       <c r="P81" s="8">
         <v>3</v>
       </c>
@@ -5078,31 +5072,31 @@
       </c>
     </row>
     <row r="82" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B82" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C82" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D82" s="16" t="s">
+      <c r="D82" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17" t="s">
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="23"/>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
       <c r="P82" s="8">
         <v>3</v>
       </c>
@@ -5117,65 +5111,65 @@
         <v>315</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A83" s="30" t="s">
+    <row r="83" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="C83" s="16" t="s">
+      <c r="C83" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E83" s="17"/>
-      <c r="F83" s="30"/>
-      <c r="G83" s="30"/>
-      <c r="H83" s="30"/>
-      <c r="I83" s="30"/>
-      <c r="J83" s="30"/>
-      <c r="K83" s="39"/>
-      <c r="L83" s="23"/>
-      <c r="M83" s="30"/>
-      <c r="N83" s="30"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="31">
-        <v>3</v>
-      </c>
-      <c r="Q83" s="32"/>
-      <c r="R83" s="33"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="K83" s="23"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="21"/>
+      <c r="N83" s="21"/>
+      <c r="O83" s="9"/>
+      <c r="P83" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q83" s="23"/>
+      <c r="R83" s="24"/>
       <c r="S83" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="T83" s="34"/>
-      <c r="U83" s="34"/>
+      <c r="T83" s="25"/>
+      <c r="U83" s="25"/>
       <c r="V83" s="9" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="17"/>
-      <c r="B84" s="20" t="s">
+    <row r="84" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="9"/>
+      <c r="B84" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="C84" s="16" t="s">
+      <c r="C84" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="D84" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="16"/>
-      <c r="L84" s="23"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
       <c r="O84" s="6"/>
       <c r="P84" s="8">
         <v>3</v>
@@ -5191,29 +5185,29 @@
         <v>315</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="58" x14ac:dyDescent="0.35">
-      <c r="A85" s="17" t="s">
+    <row r="85" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="C85" s="16" t="s">
+      <c r="C85" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="23"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
       <c r="O85" s="6"/>
       <c r="P85" s="8">
         <v>3</v>
@@ -5229,29 +5223,29 @@
         <v>315</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="17" t="s">
+    <row r="86" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="16"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
       <c r="O86" s="6"/>
       <c r="P86" s="8">
         <v>3</v>
@@ -5267,27 +5261,27 @@
         <v>315</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="17"/>
-      <c r="B87" s="20" t="s">
+    <row r="87" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="9"/>
+      <c r="B87" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="C87" s="16" t="s">
+      <c r="C87" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
       <c r="O87" s="6"/>
       <c r="P87" s="8">
         <v>3</v>
@@ -5303,29 +5297,29 @@
         <v>315</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="58" x14ac:dyDescent="0.35">
-      <c r="A88" s="17" t="s">
+    <row r="88" spans="1:22" ht="58" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="17"/>
-      <c r="K88" s="16"/>
-      <c r="L88" s="17"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
       <c r="O88" s="6"/>
       <c r="P88" s="8">
         <v>3</v>
@@ -5341,27 +5335,27 @@
         <v>315</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89" s="17"/>
-      <c r="B89" s="20" t="s">
+    <row r="89" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="9"/>
+      <c r="B89" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="17"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
       <c r="O89" s="6"/>
       <c r="P89" s="8">
         <v>3</v>
@@ -5377,29 +5371,29 @@
         <v>315</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A90" s="17" t="s">
+    <row r="90" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B90" s="20" t="s">
+      <c r="B90" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="C90" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
       <c r="O90" s="6"/>
       <c r="P90" s="8">
         <v>3</v>
@@ -5415,27 +5409,27 @@
         <v>315</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A91" s="17"/>
-      <c r="B91" s="20" t="s">
+    <row r="91" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="9"/>
+      <c r="B91" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C91" s="16" t="s">
+      <c r="C91" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="D91" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="17"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
       <c r="O91" s="6"/>
       <c r="P91" s="8">
         <v>3</v>
@@ -5451,29 +5445,29 @@
         <v>315</v>
       </c>
     </row>
-    <row r="92" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="17" t="s">
+    <row r="92" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17"/>
-      <c r="J92" s="17"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="17"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
       <c r="O92" s="6"/>
       <c r="P92" s="8">
         <v>3</v>
@@ -5489,27 +5483,27 @@
         <v>315</v>
       </c>
     </row>
-    <row r="93" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="17"/>
-      <c r="B93" s="20" t="s">
+    <row r="93" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="9"/>
+      <c r="B93" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="C93" s="16" t="s">
+      <c r="C93" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="17"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
       <c r="O93" s="6"/>
       <c r="P93" s="8">
         <v>3</v>
@@ -5525,7 +5519,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="94" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="7" t="s">
         <v>276</v>
@@ -5543,7 +5537,7 @@
       <c r="I94" s="6"/>
       <c r="J94" s="6"/>
       <c r="K94" s="7"/>
-      <c r="L94" s="23"/>
+      <c r="L94" s="6"/>
       <c r="M94" s="6"/>
       <c r="N94" s="6"/>
       <c r="O94" s="6"/>
@@ -5561,7 +5555,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="95" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="7" t="s">
         <v>278</v>
@@ -5579,7 +5573,7 @@
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
       <c r="K95" s="7"/>
-      <c r="L95" s="23"/>
+      <c r="L95" s="6"/>
       <c r="M95" s="6"/>
       <c r="N95" s="6"/>
       <c r="O95" s="6"/>
@@ -5597,8 +5591,8 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A96" s="17" t="s">
+    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -5617,7 +5611,7 @@
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="23"/>
+      <c r="L96" s="6"/>
       <c r="M96" s="6"/>
       <c r="N96" s="6"/>
       <c r="O96" s="6"/>
@@ -5635,17 +5629,17 @@
         <v>315</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:22" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C97" s="16" t="s">
+      <c r="C97" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D97" s="1" t="s">
         <v>285</v>
       </c>
       <c r="E97" s="9"/>
@@ -5655,7 +5649,7 @@
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
       <c r="K97" s="1"/>
-      <c r="L97" s="17"/>
+      <c r="L97" s="9"/>
       <c r="M97" s="9"/>
       <c r="N97" s="9"/>
       <c r="O97" s="6"/>
@@ -5673,7 +5667,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="6"/>
       <c r="B98" s="1" t="s">
         <v>148</v>
@@ -5691,7 +5685,7 @@
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="1"/>
-      <c r="L98" s="17"/>
+      <c r="L98" s="9"/>
       <c r="M98" s="9"/>
       <c r="N98" s="9"/>
       <c r="O98" s="9"/>
@@ -5710,17 +5704,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V98" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="duplicateValues" dxfId="30" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="duplicateValues" dxfId="29" priority="38"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="30" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="29" priority="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="28" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="27" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
     <cfRule type="duplicateValues" dxfId="26" priority="36"/>
@@ -5740,14 +5741,14 @@
   <conditionalFormatting sqref="B37">
     <cfRule type="duplicateValues" dxfId="21" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B99:B1048576 B1:B57 B69:B72 B75:B77 B94:B95">
-    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B73:B74">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79:B80 B82 B88">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
     <cfRule type="duplicateValues" dxfId="17" priority="13"/>
@@ -5773,35 +5774,35 @@
   <conditionalFormatting sqref="B93">
     <cfRule type="duplicateValues" dxfId="10" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79:B80 B82 B88">
-    <cfRule type="duplicateValues" dxfId="9" priority="19"/>
+  <conditionalFormatting sqref="B97">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B99:B1048576 B1:B57 B69:B72 B75:B77 B94:B95">
+    <cfRule type="duplicateValues" dxfId="8" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B99:B1048576 B1:B95">
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="duplicateValues" dxfId="7" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="5" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B99:B1048576 B1:B95">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1" xr:uid="{19E94BB0-C33D-46FC-903B-2A9BB85E51F5}"/>
@@ -5813,6 +5814,10 @@
     <hyperlink ref="L61" r:id="rId7" xr:uid="{C79858AC-5E01-4FB0-98A6-4979CC96F735}"/>
     <hyperlink ref="L67" r:id="rId8" xr:uid="{E2C83CB3-0FA9-4D6D-9E64-1BC18BF41073}"/>
     <hyperlink ref="L71" r:id="rId9" xr:uid="{ACF8DE53-589C-4E61-9BE8-6E3C9F43C69E}"/>
+    <hyperlink ref="K13" r:id="rId10" xr:uid="{1C611392-ED88-43A7-9E13-5D61817D1B01}"/>
+    <hyperlink ref="K19" r:id="rId11" xr:uid="{A1CB9838-C168-4A4D-8F54-B61550F8163D}"/>
+    <hyperlink ref="K24" r:id="rId12" xr:uid="{40886AC8-9EF7-4DAF-AC13-004D7FDD0408}"/>
+    <hyperlink ref="K21" r:id="rId13" xr:uid="{CCCDF5C0-6430-4871-831A-10911C007830}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating Intervention outcomes and spillover effects.xlsx
</commit_message>
<xml_diff>
--- a/Intervention outcomes and spillover effects/Intervention outcomes and spillover effects.xlsx
+++ b/Intervention outcomes and spillover effects/Intervention outcomes and spillover effects.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V98"/>
+  <dimension ref="A1:V99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1525,56 +1525,60 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>GMHO:0000024</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ADDICTO:0001307</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>In remission</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>A personal attribute in which the person presents fewer or lower intensity of symptoms compared to their previous symptom presentation, and the current symptoms minimally interfere with their life.</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>personal attribute</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="inlineStr"/>
-      <c r="F17" s="2" t="inlineStr"/>
-      <c r="G17" s="2" t="inlineStr"/>
-      <c r="H17" s="2" t="inlineStr"/>
-      <c r="I17" s="2" t="inlineStr"/>
-      <c r="J17" s="2" t="inlineStr"/>
-      <c r="K17" s="2" t="inlineStr"/>
-      <c r="L17" s="2" t="inlineStr"/>
-      <c r="M17" s="2" t="inlineStr"/>
-      <c r="N17" s="2" t="inlineStr"/>
-      <c r="O17" s="2" t="inlineStr"/>
-      <c r="P17" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q17" s="2" t="inlineStr">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>A health status in which the person presents fewer or lower intensity of symptoms compared to their previous symptom presentation, and the current symptoms minimally interfere with their life.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>health status</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>intervention outcomes and spillover effects</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R17" s="2" t="inlineStr"/>
-      <c r="S17" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T17" s="2" t="inlineStr"/>
-      <c r="U17" s="2" t="inlineStr"/>
-      <c r="V17" s="2" t="inlineStr">
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -4127,22 +4131,22 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>EFO:0004612</t>
+          <t>BCIO:015092</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>high density lipoprotein cholesterol measurement</t>
+          <t>health status</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>The measurement of HDL cholesterol in blood used as a risk indicator for heart disease.</t>
+          <t>A personal attribute that is the state of an individual's mental or physical condition.</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>lipid measurement</t>
+          <t>personal attribute</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -4150,17 +4154,17 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>intervention outcomes and spillover effects</t>
+        </is>
+      </c>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="P62" t="inlineStr"/>
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr"/>
       <c r="S62" t="inlineStr">
@@ -4179,31 +4183,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CHEBI:47775</t>
+          <t>EFO:0004612</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>high-density lipoprotein cholesterol</t>
+          <t>high density lipoprotein cholesterol measurement</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Cholesterol esters and free cholesterol which are contained in or bound to high-density lipoproteins (HDL).</t>
+          <t>The measurement of HDL cholesterol in blood used as a risk indicator for heart disease.</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>lipoprotein cholesterol</t>
+          <t>lipid measurement</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>HDL cholesterol</t>
-        </is>
-      </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
@@ -4233,56 +4233,56 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>GMHO:0000065</t>
-        </is>
-      </c>
-      <c r="B64" s="2" t="inlineStr">
-        <is>
-          <t>homicide following an intervention</t>
-        </is>
-      </c>
-      <c r="C64" s="2" t="inlineStr">
-        <is>
-          <t>A death following an intervention that involves a participant being intentionally killed by another person.</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="inlineStr">
-        <is>
-          <t>death following an intervention</t>
-        </is>
-      </c>
-      <c r="E64" s="2" t="inlineStr"/>
-      <c r="F64" s="2" t="inlineStr"/>
-      <c r="G64" s="2" t="inlineStr"/>
-      <c r="H64" s="2" t="inlineStr"/>
-      <c r="I64" s="2" t="inlineStr"/>
-      <c r="J64" s="2" t="inlineStr"/>
-      <c r="K64" s="2" t="inlineStr"/>
-      <c r="L64" s="2" t="inlineStr"/>
-      <c r="M64" s="2" t="inlineStr"/>
-      <c r="N64" s="2" t="inlineStr"/>
-      <c r="O64" s="2" t="inlineStr"/>
-      <c r="P64" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q64" s="2" t="inlineStr">
-        <is>
-          <t>Intervention outcomes and spillover effects</t>
-        </is>
-      </c>
-      <c r="R64" s="2" t="inlineStr"/>
-      <c r="S64" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T64" s="2" t="inlineStr"/>
-      <c r="U64" s="2" t="inlineStr"/>
-      <c r="V64" s="2" t="inlineStr">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CHEBI:47775</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>high-density lipoprotein cholesterol</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Cholesterol esters and free cholesterol which are contained in or bound to high-density lipoproteins (HDL).</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>lipoprotein cholesterol</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>HDL cholesterol</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -4291,22 +4291,22 @@
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000066</t>
+          <t>GMHO:0000065</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>hospitalization</t>
+          <t>homicide following an intervention</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>A health care process that involves a person being admitted to a hospital.</t>
+          <t>A death following an intervention that involves a participant being intentionally killed by another person.</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
         <is>
-          <t>health care process</t>
+          <t>death following an intervention</t>
         </is>
       </c>
       <c r="E65" s="2" t="inlineStr"/>
@@ -4316,11 +4316,7 @@
       <c r="I65" s="2" t="inlineStr"/>
       <c r="J65" s="2" t="inlineStr"/>
       <c r="K65" s="2" t="inlineStr"/>
-      <c r="L65" s="2" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/OGMS_0000098</t>
-        </is>
-      </c>
+      <c r="L65" s="2" t="inlineStr"/>
       <c r="M65" s="2" t="inlineStr"/>
       <c r="N65" s="2" t="inlineStr"/>
       <c r="O65" s="2" t="inlineStr"/>
@@ -4351,22 +4347,22 @@
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000067</t>
+          <t>GMHO:0000066</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>human functioning</t>
+          <t>hospitalization</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>A bodily disposition to realise processes that influence a person's life quality.</t>
+          <t>A health care process that involves a person being admitted to a hospital.</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
-          <t>bodily disposition</t>
+          <t>health care process</t>
         </is>
       </c>
       <c r="E66" s="2" t="inlineStr"/>
@@ -4376,7 +4372,11 @@
       <c r="I66" s="2" t="inlineStr"/>
       <c r="J66" s="2" t="inlineStr"/>
       <c r="K66" s="2" t="inlineStr"/>
-      <c r="L66" s="2" t="inlineStr"/>
+      <c r="L66" s="2" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/OGMS_0000098</t>
+        </is>
+      </c>
       <c r="M66" s="2" t="inlineStr"/>
       <c r="N66" s="2" t="inlineStr"/>
       <c r="O66" s="2" t="inlineStr"/>
@@ -4405,56 +4405,56 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>BCIO:017000</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>intervention effect estimate</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>An intervention evaluation finding that characterises the difference between intervention outcome estimates of two intervention scenarios.</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>intervention evaluation finding</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr"/>
-      <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr"/>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000067</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>human functioning</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>A bodily disposition to realise processes that influence a person's life quality.</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>bodily disposition</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr"/>
+      <c r="F67" s="2" t="inlineStr"/>
+      <c r="G67" s="2" t="inlineStr"/>
+      <c r="H67" s="2" t="inlineStr"/>
+      <c r="I67" s="2" t="inlineStr"/>
+      <c r="J67" s="2" t="inlineStr"/>
+      <c r="K67" s="2" t="inlineStr"/>
+      <c r="L67" s="2" t="inlineStr"/>
+      <c r="M67" s="2" t="inlineStr"/>
+      <c r="N67" s="2" t="inlineStr"/>
+      <c r="O67" s="2" t="inlineStr"/>
+      <c r="P67" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q67" s="2" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R67" t="inlineStr"/>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="T67" t="inlineStr"/>
-      <c r="U67" t="inlineStr"/>
-      <c r="V67" t="inlineStr">
+      <c r="R67" s="2" t="inlineStr"/>
+      <c r="S67" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T67" s="2" t="inlineStr"/>
+      <c r="U67" s="2" t="inlineStr"/>
+      <c r="V67" s="2" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -4463,22 +4463,22 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BCIO:023000</t>
+          <t>BCIO:017000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>intervention effect estimate</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>An intervention evaluation finding that characterises the difference between intervention outcome estimates of two intervention scenarios.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
           <t>intervention evaluation finding</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>An evaluation finding that is the output of an intervention evaluation study.</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>evaluation finding</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -4517,108 +4517,112 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="inlineStr">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>BCIO:023000</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>intervention evaluation finding</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>An evaluation finding that is the output of an intervention evaluation study.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>evaluation finding</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>Intervention outcomes and spillover effects</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr"/>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
         <is>
           <t>GMHO:0000068</t>
         </is>
       </c>
-      <c r="B69" s="2" t="inlineStr">
+      <c r="B70" s="2" t="inlineStr">
         <is>
           <t>intervention outcome</t>
         </is>
       </c>
-      <c r="C69" s="2" t="inlineStr">
+      <c r="C70" s="2" t="inlineStr">
         <is>
           <t>A process that is influenced by an intervention.</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr">
+      <c r="D70" s="2" t="inlineStr">
         <is>
           <t>process</t>
         </is>
       </c>
-      <c r="E69" s="2" t="inlineStr"/>
-      <c r="F69" s="2" t="inlineStr"/>
-      <c r="G69" s="2" t="inlineStr"/>
-      <c r="H69" s="2" t="inlineStr"/>
-      <c r="I69" s="2" t="inlineStr"/>
-      <c r="J69" s="2" t="inlineStr"/>
-      <c r="K69" s="2" t="inlineStr"/>
-      <c r="L69" s="2" t="inlineStr"/>
-      <c r="M69" s="2" t="inlineStr"/>
-      <c r="N69" s="2" t="inlineStr"/>
-      <c r="O69" s="2" t="inlineStr"/>
-      <c r="P69" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q69" s="2" t="inlineStr">
+      <c r="E70" s="2" t="inlineStr"/>
+      <c r="F70" s="2" t="inlineStr"/>
+      <c r="G70" s="2" t="inlineStr"/>
+      <c r="H70" s="2" t="inlineStr"/>
+      <c r="I70" s="2" t="inlineStr"/>
+      <c r="J70" s="2" t="inlineStr"/>
+      <c r="K70" s="2" t="inlineStr"/>
+      <c r="L70" s="2" t="inlineStr"/>
+      <c r="M70" s="2" t="inlineStr"/>
+      <c r="N70" s="2" t="inlineStr"/>
+      <c r="O70" s="2" t="inlineStr"/>
+      <c r="P70" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q70" s="2" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R69" s="2" t="inlineStr"/>
-      <c r="S69" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T69" s="2" t="inlineStr"/>
-      <c r="U69" s="2" t="inlineStr"/>
-      <c r="V69" s="2" t="inlineStr">
-        <is>
-          <t>PS</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>EFO:0004611</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>low density lipoprotein cholesterol measurement</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>The measurement of LDL cholesterol in blood used as a risk indicator for heart disease.</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>lipid measurement</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr"/>
-      <c r="O70" t="inlineStr"/>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q70" t="inlineStr"/>
-      <c r="R70" t="inlineStr"/>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="T70" t="inlineStr"/>
-      <c r="U70" t="inlineStr"/>
-      <c r="V70" t="inlineStr">
+      <c r="R70" s="2" t="inlineStr"/>
+      <c r="S70" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T70" s="2" t="inlineStr"/>
+      <c r="U70" s="2" t="inlineStr"/>
+      <c r="V70" s="2" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -4627,31 +4631,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CHEBI:47774</t>
+          <t>EFO:0004611</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>low-density lipoprotein cholesterol</t>
+          <t>low density lipoprotein cholesterol measurement</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Cholesterol esters and free cholesterol which are contained in or bound to low-density lipoproteins (LDL).</t>
+          <t>The measurement of LDL cholesterol in blood used as a risk indicator for heart disease.</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>lipoprotein cholesterol</t>
+          <t>lipid measurement</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>LDL cholesterol</t>
-        </is>
-      </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
@@ -4683,27 +4683,31 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>IAO:0000109</t>
+          <t>CHEBI:47774</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>measurement data item</t>
+          <t>low-density lipoprotein cholesterol</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>A data item that is a recording of the output of an assay.</t>
+          <t>Cholesterol esters and free cholesterol which are contained in or bound to low-density lipoproteins (LDL).</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>lipoprotein cholesterol</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>LDL cholesterol</t>
+        </is>
+      </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
@@ -4717,11 +4721,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>Intervention outcomes and spillover effects</t>
-        </is>
-      </c>
+      <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
       <c r="S72" t="inlineStr">
         <is>
@@ -4739,22 +4739,22 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MF:0000000</t>
+          <t>IAO:0000109</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>mental functioning related anatomical structure</t>
+          <t>measurement data item</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>An anatomical structure in which there inheres the disposition to be the agent of a mental process.</t>
+          <t>A data item that is a recording of the output of an assay.</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>fiat object part</t>
+          <t>data item</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -4793,60 +4793,56 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="inlineStr">
-        <is>
-          <t>GMHO:0000069</t>
-        </is>
-      </c>
-      <c r="B74" s="2" t="inlineStr">
-        <is>
-          <t>negative psychotic disorder symptom</t>
-        </is>
-      </c>
-      <c r="C74" s="2" t="inlineStr">
-        <is>
-          <t>A psychotic disorder symptom that is characterized by the absence or decrease in ability or motivation to initiate plans, speak, express emotion of find pleasure.</t>
-        </is>
-      </c>
-      <c r="D74" s="2" t="inlineStr">
-        <is>
-          <t>psychotic disorder symptom</t>
-        </is>
-      </c>
-      <c r="E74" s="2" t="inlineStr"/>
-      <c r="F74" s="2" t="inlineStr"/>
-      <c r="G74" s="2" t="inlineStr"/>
-      <c r="H74" s="2" t="inlineStr"/>
-      <c r="I74" s="2" t="inlineStr"/>
-      <c r="J74" s="2" t="inlineStr"/>
-      <c r="K74" s="2" t="inlineStr">
-        <is>
-          <t>Based on https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia</t>
-        </is>
-      </c>
-      <c r="L74" s="2" t="inlineStr"/>
-      <c r="M74" s="2" t="inlineStr"/>
-      <c r="N74" s="2" t="inlineStr"/>
-      <c r="O74" s="2" t="inlineStr"/>
-      <c r="P74" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q74" s="2" t="inlineStr">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>MF:0000000</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>mental functioning related anatomical structure</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>An anatomical structure in which there inheres the disposition to be the agent of a mental process.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>fiat object part</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R74" s="2" t="inlineStr"/>
-      <c r="S74" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T74" s="2" t="inlineStr"/>
-      <c r="U74" s="2" t="inlineStr"/>
-      <c r="V74" s="2" t="inlineStr">
+      <c r="R74" t="inlineStr"/>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -4855,22 +4851,22 @@
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000070</t>
+          <t>GMHO:0000069</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>negative psychotic disorder symptom severity</t>
+          <t>negative psychotic disorder symptom</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>Psychotic disorder symptom severity that is associated with negative psychotic disorder symptoms.</t>
+          <t>A psychotic disorder symptom that is characterized by the absence or decrease in ability or motivation to initiate plans, speak, express emotion of find pleasure.</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>psychotic disorder symptom severity</t>
+          <t>psychotic disorder symptom</t>
         </is>
       </c>
       <c r="E75" s="2" t="inlineStr"/>
@@ -4879,7 +4875,11 @@
       <c r="H75" s="2" t="inlineStr"/>
       <c r="I75" s="2" t="inlineStr"/>
       <c r="J75" s="2" t="inlineStr"/>
-      <c r="K75" s="2" t="inlineStr"/>
+      <c r="K75" s="2" t="inlineStr">
+        <is>
+          <t>Based on https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia</t>
+        </is>
+      </c>
       <c r="L75" s="2" t="inlineStr"/>
       <c r="M75" s="2" t="inlineStr"/>
       <c r="N75" s="2" t="inlineStr"/>
@@ -4911,22 +4911,22 @@
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000071</t>
+          <t>GMHO:0000070</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuroleptic-induced parkinsonism following intervention </t>
+          <t>negative psychotic disorder symptom severity</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>A drug-induced movement disorder following intervention that involves experiencing slowness of movement, tremors and rigidity.</t>
+          <t>Psychotic disorder symptom severity that is associated with negative psychotic disorder symptoms.</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
-          <t>drug-induced movement disorder following intervention</t>
+          <t>psychotic disorder symptom severity</t>
         </is>
       </c>
       <c r="E76" s="2" t="inlineStr"/>
@@ -4935,11 +4935,7 @@
       <c r="H76" s="2" t="inlineStr"/>
       <c r="I76" s="2" t="inlineStr"/>
       <c r="J76" s="2" t="inlineStr"/>
-      <c r="K76" s="2" t="inlineStr">
-        <is>
-          <t>Based on https://link.springer.com/article/10.1007/s007020100006</t>
-        </is>
-      </c>
+      <c r="K76" s="2" t="inlineStr"/>
       <c r="L76" s="2" t="inlineStr"/>
       <c r="M76" s="2" t="inlineStr"/>
       <c r="N76" s="2" t="inlineStr"/>
@@ -4949,7 +4945,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q76" s="2" t="inlineStr"/>
+      <c r="Q76" s="2" t="inlineStr">
+        <is>
+          <t>Intervention outcomes and spillover effects</t>
+        </is>
+      </c>
       <c r="R76" s="2" t="inlineStr"/>
       <c r="S76" s="2" t="inlineStr">
         <is>
@@ -4967,22 +4967,22 @@
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000072</t>
+          <t>GMHO:0000071</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out due to adverse events</t>
+          <t xml:space="preserve">neuroleptic-induced parkinsonism following intervention </t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>Number of participant drop-out from the intervention as a result the participants experiencing some adverse event.</t>
+          <t>A drug-induced movement disorder following intervention that involves experiencing slowness of movement, tremors and rigidity.</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out from intervention</t>
+          <t>drug-induced movement disorder following intervention</t>
         </is>
       </c>
       <c r="E77" s="2" t="inlineStr"/>
@@ -4991,7 +4991,11 @@
       <c r="H77" s="2" t="inlineStr"/>
       <c r="I77" s="2" t="inlineStr"/>
       <c r="J77" s="2" t="inlineStr"/>
-      <c r="K77" s="2" t="inlineStr"/>
+      <c r="K77" s="2" t="inlineStr">
+        <is>
+          <t>Based on https://link.springer.com/article/10.1007/s007020100006</t>
+        </is>
+      </c>
       <c r="L77" s="2" t="inlineStr"/>
       <c r="M77" s="2" t="inlineStr"/>
       <c r="N77" s="2" t="inlineStr"/>
@@ -5001,11 +5005,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q77" s="2" t="inlineStr">
-        <is>
-          <t>Intervention outcomes and spillover effects</t>
-        </is>
-      </c>
+      <c r="Q77" s="2" t="inlineStr"/>
       <c r="R77" s="2" t="inlineStr"/>
       <c r="S77" s="2" t="inlineStr">
         <is>
@@ -5023,17 +5023,17 @@
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000073</t>
+          <t>GMHO:0000072</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out due to inefficacy</t>
+          <t>number of participant drop-out due to adverse events</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>Number of participant drop-out from the intervention as a result of the intervention failing to produce the desired effect.</t>
+          <t>Number of participant drop-out from the intervention as a result the participants experiencing some adverse event.</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -5079,22 +5079,22 @@
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000074</t>
+          <t>GMHO:0000073</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out due to side-events</t>
+          <t>number of participant drop-out due to inefficacy</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>Number of participant drop-out due to adverse events that are experienced following the intervention.</t>
+          <t>Number of participant drop-out from the intervention as a result of the intervention failing to produce the desired effect.</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out due to adverse events</t>
+          <t>number of participant drop-out from intervention</t>
         </is>
       </c>
       <c r="E79" s="2" t="inlineStr"/>
@@ -5135,22 +5135,22 @@
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000075</t>
+          <t>GMHO:0000074</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>number of participant drop-out from intervention</t>
+          <t>number of participant drop-out due to side-events</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>Number of intervention participants who withdraw from or cannot complete an intervention.</t>
+          <t>Number of participant drop-out due to adverse events that are experienced following the intervention.</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
         <is>
-          <t>number of intervention participants</t>
+          <t>number of participant drop-out due to adverse events</t>
         </is>
       </c>
       <c r="E80" s="2" t="inlineStr"/>
@@ -5191,22 +5191,22 @@
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000076</t>
+          <t>GMHO:0000075</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>positive intervention outcome</t>
+          <t>number of participant drop-out from intervention</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">An intervention outcome that is positively influenced by the intervention. </t>
+          <t>Number of intervention participants who withdraw from or cannot complete an intervention.</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr">
         <is>
-          <t>intervention outcome</t>
+          <t>number of intervention participants</t>
         </is>
       </c>
       <c r="E81" s="2" t="inlineStr"/>
@@ -5247,22 +5247,22 @@
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000077</t>
+          <t>GMHO:0000076</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>positive psychotic disorder symptom</t>
+          <t>positive intervention outcome</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>A psychotic disorder symptom that is characterized by the presence of hallucinations, delusions, or disorganised thoughts or behaviours.</t>
+          <t xml:space="preserve">An intervention outcome that is positively influenced by the intervention. </t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>psychotic disorder symptom</t>
+          <t>intervention outcome</t>
         </is>
       </c>
       <c r="E82" s="2" t="inlineStr"/>
@@ -5271,11 +5271,7 @@
       <c r="H82" s="2" t="inlineStr"/>
       <c r="I82" s="2" t="inlineStr"/>
       <c r="J82" s="2" t="inlineStr"/>
-      <c r="K82" s="2" t="inlineStr">
-        <is>
-          <t>Based on https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia</t>
-        </is>
-      </c>
+      <c r="K82" s="2" t="inlineStr"/>
       <c r="L82" s="2" t="inlineStr"/>
       <c r="M82" s="2" t="inlineStr"/>
       <c r="N82" s="2" t="inlineStr"/>
@@ -5307,22 +5303,22 @@
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000078</t>
+          <t>GMHO:0000077</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>positive psychotic disorder symptom severity</t>
+          <t>positive psychotic disorder symptom</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>Psychotic disorder symptom severity that is associated with positive psychotic disorder symptoms.</t>
+          <t>A psychotic disorder symptom that is characterized by the presence of hallucinations, delusions, or disorganised thoughts or behaviours.</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
-          <t>psychotic disorder symptom severity</t>
+          <t>psychotic disorder symptom</t>
         </is>
       </c>
       <c r="E83" s="2" t="inlineStr"/>
@@ -5331,7 +5327,11 @@
       <c r="H83" s="2" t="inlineStr"/>
       <c r="I83" s="2" t="inlineStr"/>
       <c r="J83" s="2" t="inlineStr"/>
-      <c r="K83" s="2" t="inlineStr"/>
+      <c r="K83" s="2" t="inlineStr">
+        <is>
+          <t>Based on https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia</t>
+        </is>
+      </c>
       <c r="L83" s="2" t="inlineStr"/>
       <c r="M83" s="2" t="inlineStr"/>
       <c r="N83" s="2" t="inlineStr"/>
@@ -5346,11 +5346,7 @@
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R83" s="2" t="inlineStr">
-        <is>
-          <t>A measure for 'positive psychotic disorder symptom severity'</t>
-        </is>
-      </c>
+      <c r="R83" s="2" t="inlineStr"/>
       <c r="S83" s="2" t="inlineStr">
         <is>
           <t>Proposed</t>
@@ -5365,52 +5361,60 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>EFO:0007003</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>prolactin measurement</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Quantification of prolactin in a sample.</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>hormone measurement</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr"/>
-      <c r="P84" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q84" t="inlineStr"/>
-      <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="T84" t="inlineStr"/>
-      <c r="U84" t="inlineStr"/>
-      <c r="V84" t="inlineStr">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000078</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>positive psychotic disorder symptom severity</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>Psychotic disorder symptom severity that is associated with positive psychotic disorder symptoms.</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>psychotic disorder symptom severity</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr"/>
+      <c r="F84" s="2" t="inlineStr"/>
+      <c r="G84" s="2" t="inlineStr"/>
+      <c r="H84" s="2" t="inlineStr"/>
+      <c r="I84" s="2" t="inlineStr"/>
+      <c r="J84" s="2" t="inlineStr"/>
+      <c r="K84" s="2" t="inlineStr"/>
+      <c r="L84" s="2" t="inlineStr"/>
+      <c r="M84" s="2" t="inlineStr"/>
+      <c r="N84" s="2" t="inlineStr"/>
+      <c r="O84" s="2" t="inlineStr"/>
+      <c r="P84" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q84" s="2" t="inlineStr">
+        <is>
+          <t>Intervention outcomes and spillover effects</t>
+        </is>
+      </c>
+      <c r="R84" s="2" t="inlineStr">
+        <is>
+          <t>A measure for 'positive psychotic disorder symptom severity'</t>
+        </is>
+      </c>
+      <c r="S84" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T84" s="2" t="inlineStr"/>
+      <c r="U84" s="2" t="inlineStr"/>
+      <c r="V84" s="2" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -5419,29 +5423,25 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>OGMS:0000020</t>
+          <t>EFO:0007003</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>psychotic disorder symptom</t>
+          <t>prolactin measurement</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>A symptom that is related to a psychotic disorder diagnosis.</t>
+          <t>Quantification of prolactin in a sample.</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>symptom</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/</t>
-        </is>
-      </c>
+          <t>hormone measurement</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
@@ -5457,11 +5457,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>Intervention outcomes and spillover effects</t>
-        </is>
-      </c>
+      <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr"/>
       <c r="S85" t="inlineStr">
         <is>
@@ -5477,56 +5473,60 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="inlineStr">
-        <is>
-          <t>GMHO:0000079</t>
-        </is>
-      </c>
-      <c r="B86" s="2" t="inlineStr">
-        <is>
-          <t>psychotic disorder symptom severity</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="inlineStr">
-        <is>
-          <t>Symptom severity that is associated with a psychotic disorder symptom.</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="inlineStr">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>OGMS:0000020</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
         <is>
           <t>psychotic disorder symptom</t>
         </is>
       </c>
-      <c r="E86" s="2" t="inlineStr"/>
-      <c r="F86" s="2" t="inlineStr"/>
-      <c r="G86" s="2" t="inlineStr"/>
-      <c r="H86" s="2" t="inlineStr"/>
-      <c r="I86" s="2" t="inlineStr"/>
-      <c r="J86" s="2" t="inlineStr"/>
-      <c r="K86" s="2" t="inlineStr"/>
-      <c r="L86" s="2" t="inlineStr"/>
-      <c r="M86" s="2" t="inlineStr"/>
-      <c r="N86" s="2" t="inlineStr"/>
-      <c r="O86" s="2" t="inlineStr"/>
-      <c r="P86" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q86" s="2" t="inlineStr">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>A symptom that is related to a psychotic disorder diagnosis.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>symptom</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q86" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R86" s="2" t="inlineStr"/>
-      <c r="S86" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T86" s="2" t="inlineStr"/>
-      <c r="U86" s="2" t="inlineStr"/>
-      <c r="V86" s="2" t="inlineStr">
+      <c r="R86" t="inlineStr"/>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T86" t="inlineStr"/>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -5535,22 +5535,22 @@
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000080</t>
+          <t>GMHO:0000079</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>relapsed</t>
+          <t>psychotic disorder symptom severity</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>A personal attribute in which the person's symptoms have reverted temporarily from a more desired level to their previous severity.</t>
+          <t>Symptom severity that is associated with a psychotic disorder symptom.</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>personal attribute</t>
+          <t>psychotic disorder symptom</t>
         </is>
       </c>
       <c r="E87" s="2" t="inlineStr"/>
@@ -5589,64 +5589,60 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="inlineStr">
-        <is>
-          <t>GMHO:0000081</t>
-        </is>
-      </c>
-      <c r="B88" s="2" t="inlineStr">
-        <is>
-          <t>serious adverse event following an intervention</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>An adverse event following an intervention that results in death, a life-threatening event, a persistent or significant disability or a birth defect or requires hospitalisation or extends hospitalisation.</t>
-        </is>
-      </c>
-      <c r="D88" s="2" t="inlineStr">
-        <is>
-          <t>adverse event following an intervention</t>
-        </is>
-      </c>
-      <c r="E88" s="2" t="inlineStr"/>
-      <c r="F88" s="2" t="inlineStr"/>
-      <c r="G88" s="2" t="inlineStr"/>
-      <c r="H88" s="2" t="inlineStr"/>
-      <c r="I88" s="2" t="inlineStr"/>
-      <c r="J88" s="2" t="inlineStr"/>
-      <c r="K88" s="2" t="inlineStr">
-        <is>
-          <t>Based on http://purl.obolibrary.org/obo/OAE_0000631</t>
-        </is>
-      </c>
-      <c r="L88" s="2" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/OAE_0000631</t>
-        </is>
-      </c>
-      <c r="M88" s="2" t="inlineStr"/>
-      <c r="N88" s="2" t="inlineStr"/>
-      <c r="O88" s="2" t="inlineStr"/>
-      <c r="P88" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q88" s="2" t="inlineStr">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ADDICTO:0001308</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>relapsed</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>A health status in which the symptoms of a person suffering from a disorder have reverted from a desired level to an undesired level.</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>health status</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>intervention outcomes and spillover effects</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q88" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R88" s="2" t="inlineStr"/>
-      <c r="S88" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T88" s="2" t="inlineStr"/>
-      <c r="U88" s="2" t="inlineStr"/>
-      <c r="V88" s="2" t="inlineStr">
+      <c r="R88" t="inlineStr"/>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="inlineStr"/>
+      <c r="V88" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -5655,22 +5651,22 @@
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000082</t>
+          <t>GMHO:0000081</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>serious psychological adverse event following an intervention</t>
+          <t>serious adverse event following an intervention</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>A serious adverse event following an intervention that is associated with multiple, persistent or salient negative mental processes.</t>
+          <t>An adverse event following an intervention that results in death, a life-threatening event, a persistent or significant disability or a birth defect or requires hospitalisation or extends hospitalisation.</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>serious adverse event following an intervention</t>
+          <t>adverse event following an intervention</t>
         </is>
       </c>
       <c r="E89" s="2" t="inlineStr"/>
@@ -5679,8 +5675,16 @@
       <c r="H89" s="2" t="inlineStr"/>
       <c r="I89" s="2" t="inlineStr"/>
       <c r="J89" s="2" t="inlineStr"/>
-      <c r="K89" s="2" t="inlineStr"/>
-      <c r="L89" s="2" t="inlineStr"/>
+      <c r="K89" s="2" t="inlineStr">
+        <is>
+          <t>Based on http://purl.obolibrary.org/obo/OAE_0000631</t>
+        </is>
+      </c>
+      <c r="L89" s="2" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/OAE_0000631</t>
+        </is>
+      </c>
       <c r="M89" s="2" t="inlineStr"/>
       <c r="N89" s="2" t="inlineStr"/>
       <c r="O89" s="2" t="inlineStr"/>
@@ -5711,17 +5715,17 @@
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000083</t>
+          <t>GMHO:0000082</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>serious somatic adverse event following an intervention</t>
+          <t>serious psychological adverse event following an intervention</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>A serious adverse event following an intervention that is associated with multiple, persistent or salient physical symptoms.</t>
+          <t>A serious adverse event following an intervention that is associated with multiple, persistent or salient negative mental processes.</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
@@ -5767,22 +5771,22 @@
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000084</t>
+          <t>GMHO:0000083</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>suicidal ideation following intervention</t>
+          <t>serious somatic adverse event following an intervention</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>An adverse event following an intervention that involves thoughts about suicide.</t>
+          <t>A serious adverse event following an intervention that is associated with multiple, persistent or salient physical symptoms.</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr">
         <is>
-          <t>adverse event following an intervention</t>
+          <t>serious adverse event following an intervention</t>
         </is>
       </c>
       <c r="E91" s="2" t="inlineStr"/>
@@ -5791,16 +5795,8 @@
       <c r="H91" s="2" t="inlineStr"/>
       <c r="I91" s="2" t="inlineStr"/>
       <c r="J91" s="2" t="inlineStr"/>
-      <c r="K91" s="2" t="inlineStr">
-        <is>
-          <t>Based on http://purl.obolibrary.org/obo/OAE_0001432</t>
-        </is>
-      </c>
-      <c r="L91" s="2" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/OAE_0001432</t>
-        </is>
-      </c>
+      <c r="K91" s="2" t="inlineStr"/>
+      <c r="L91" s="2" t="inlineStr"/>
       <c r="M91" s="2" t="inlineStr"/>
       <c r="N91" s="2" t="inlineStr"/>
       <c r="O91" s="2" t="inlineStr"/>
@@ -5831,17 +5827,17 @@
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000085</t>
+          <t>GMHO:0000084</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>suicide attempt following intervention</t>
+          <t>suicidal ideation following intervention</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>An adverse event following an intervention that involves at least one attempted suicide.</t>
+          <t>An adverse event following an intervention that involves thoughts about suicide.</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
@@ -5857,12 +5853,12 @@
       <c r="J92" s="2" t="inlineStr"/>
       <c r="K92" s="2" t="inlineStr">
         <is>
-          <t>Based on http://purl.obolibrary.org/obo/OAE_0001433</t>
+          <t>Based on http://purl.obolibrary.org/obo/OAE_0001432</t>
         </is>
       </c>
       <c r="L92" s="2" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/OAE_0001433</t>
+          <t>http://purl.obolibrary.org/obo/OAE_0001432</t>
         </is>
       </c>
       <c r="M92" s="2" t="inlineStr"/>
@@ -5895,22 +5891,22 @@
     <row r="93">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000086</t>
+          <t>GMHO:0000085</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>suicide following an intervention</t>
+          <t>suicide attempt following intervention</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>A death following an intervention that involves a participant intentionally ending their own life.</t>
+          <t>An adverse event following an intervention that involves at least one attempted suicide.</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr">
         <is>
-          <t>death following an intervention</t>
+          <t>adverse event following an intervention</t>
         </is>
       </c>
       <c r="E93" s="2" t="inlineStr"/>
@@ -5919,8 +5915,16 @@
       <c r="H93" s="2" t="inlineStr"/>
       <c r="I93" s="2" t="inlineStr"/>
       <c r="J93" s="2" t="inlineStr"/>
-      <c r="K93" s="2" t="inlineStr"/>
-      <c r="L93" s="2" t="inlineStr"/>
+      <c r="K93" s="2" t="inlineStr">
+        <is>
+          <t>Based on http://purl.obolibrary.org/obo/OAE_0001433</t>
+        </is>
+      </c>
+      <c r="L93" s="2" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/OAE_0001433</t>
+        </is>
+      </c>
       <c r="M93" s="2" t="inlineStr"/>
       <c r="N93" s="2" t="inlineStr"/>
       <c r="O93" s="2" t="inlineStr"/>
@@ -5951,22 +5955,22 @@
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>GMHO:0000087</t>
+          <t>GMHO:0000086</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>symptom severity</t>
+          <t>suicide following an intervention</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>A data item that is about the severity dimension associated with a symptom.</t>
+          <t>A death following an intervention that involves a participant intentionally ending their own life.</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>death following an intervention</t>
         </is>
       </c>
       <c r="E94" s="2" t="inlineStr"/>
@@ -5990,11 +5994,7 @@
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R94" s="2" t="inlineStr">
-        <is>
-          <t>A measure for 'psychotic disorder symptom severity'</t>
-        </is>
-      </c>
+      <c r="R94" s="2" t="inlineStr"/>
       <c r="S94" s="2" t="inlineStr">
         <is>
           <t>Proposed</t>
@@ -6009,52 +6009,60 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>EFO:0004574</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>total cholesterol measurement</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>A total cholesterol measurement is the quantification of cholesterol in blood, total cholesterol is defined as the sum of HDL, LDL, and VLDL.</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>lipid measurement</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q95" t="inlineStr"/>
-      <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="T95" t="inlineStr"/>
-      <c r="U95" t="inlineStr"/>
-      <c r="V95" t="inlineStr">
+      <c r="A95" s="2" t="inlineStr">
+        <is>
+          <t>GMHO:0000087</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="inlineStr">
+        <is>
+          <t>symptom severity</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>A data item that is about the severity dimension associated with a symptom.</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>data item</t>
+        </is>
+      </c>
+      <c r="E95" s="2" t="inlineStr"/>
+      <c r="F95" s="2" t="inlineStr"/>
+      <c r="G95" s="2" t="inlineStr"/>
+      <c r="H95" s="2" t="inlineStr"/>
+      <c r="I95" s="2" t="inlineStr"/>
+      <c r="J95" s="2" t="inlineStr"/>
+      <c r="K95" s="2" t="inlineStr"/>
+      <c r="L95" s="2" t="inlineStr"/>
+      <c r="M95" s="2" t="inlineStr"/>
+      <c r="N95" s="2" t="inlineStr"/>
+      <c r="O95" s="2" t="inlineStr"/>
+      <c r="P95" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q95" s="2" t="inlineStr">
+        <is>
+          <t>Intervention outcomes and spillover effects</t>
+        </is>
+      </c>
+      <c r="R95" s="2" t="inlineStr">
+        <is>
+          <t>A measure for 'psychotic disorder symptom severity'</t>
+        </is>
+      </c>
+      <c r="S95" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T95" s="2" t="inlineStr"/>
+      <c r="U95" s="2" t="inlineStr"/>
+      <c r="V95" s="2" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
@@ -6063,17 +6071,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>EFO:0004530</t>
+          <t>EFO:0004574</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>triglyceride measurement</t>
+          <t>total cholesterol measurement</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>A triglyceride measurement is a quantification of triglycerides in some body fluid, used as a biomarker for cardiovascular disease.</t>
+          <t>A total cholesterol measurement is the quantification of cholesterol in blood, total cholesterol is defined as the sum of HDL, LDL, and VLDL.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -6113,108 +6121,160 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="inlineStr">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>EFO:0004530</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>triglyceride measurement</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>A triglyceride measurement is a quantification of triglycerides in some body fluid, used as a biomarker for cardiovascular disease.</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>lipid measurement</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q97" t="inlineStr"/>
+      <c r="R97" t="inlineStr"/>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="T97" t="inlineStr"/>
+      <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>GMHO:0000088</t>
         </is>
       </c>
-      <c r="B97" s="2" t="inlineStr">
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>unnatural dealth due to external factors following an intervention</t>
         </is>
       </c>
-      <c r="C97" s="2" t="inlineStr">
+      <c r="C98" s="2" t="inlineStr">
         <is>
           <t>homicide following an intervention' OR 'death due to accidents following an intervention'</t>
         </is>
       </c>
-      <c r="D97" s="2" t="inlineStr">
+      <c r="D98" s="2" t="inlineStr">
         <is>
           <t>death following an intervention</t>
         </is>
       </c>
-      <c r="E97" s="2" t="inlineStr"/>
-      <c r="F97" s="2" t="inlineStr"/>
-      <c r="G97" s="2" t="inlineStr"/>
-      <c r="H97" s="2" t="inlineStr"/>
-      <c r="I97" s="2" t="inlineStr"/>
-      <c r="J97" s="2" t="inlineStr"/>
-      <c r="K97" s="2" t="inlineStr"/>
-      <c r="L97" s="2" t="inlineStr"/>
-      <c r="M97" s="2" t="inlineStr"/>
-      <c r="N97" s="2" t="inlineStr"/>
-      <c r="O97" s="2" t="inlineStr"/>
-      <c r="P97" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q97" s="2" t="inlineStr">
+      <c r="E98" s="2" t="inlineStr"/>
+      <c r="F98" s="2" t="inlineStr"/>
+      <c r="G98" s="2" t="inlineStr"/>
+      <c r="H98" s="2" t="inlineStr"/>
+      <c r="I98" s="2" t="inlineStr"/>
+      <c r="J98" s="2" t="inlineStr"/>
+      <c r="K98" s="2" t="inlineStr"/>
+      <c r="L98" s="2" t="inlineStr"/>
+      <c r="M98" s="2" t="inlineStr"/>
+      <c r="N98" s="2" t="inlineStr"/>
+      <c r="O98" s="2" t="inlineStr"/>
+      <c r="P98" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q98" s="2" t="inlineStr">
         <is>
           <t>Intervention outcomes and spillover effects</t>
         </is>
       </c>
-      <c r="R97" s="2" t="inlineStr"/>
-      <c r="S97" s="2" t="inlineStr">
-        <is>
-          <t>Proposed</t>
-        </is>
-      </c>
-      <c r="T97" s="2" t="inlineStr"/>
-      <c r="U97" s="2" t="inlineStr"/>
-      <c r="V97" s="2" t="inlineStr">
-        <is>
-          <t>PS</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="R98" s="2" t="inlineStr"/>
+      <c r="S98" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="T98" s="2" t="inlineStr"/>
+      <c r="U98" s="2" t="inlineStr"/>
+      <c r="V98" s="2" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
         <is>
           <t>CHEBI:47773</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B99" t="inlineStr">
         <is>
           <t>very-low-density lipoprotein cholesterol</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>Cholesterol esters and free cholesterol which are contained in or bound to very low density lipoproteins (VLDL).</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
+      <c r="D99" t="inlineStr">
         <is>
           <t>lipoprotein cholesterol</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q98" t="inlineStr"/>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr">
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
+      <c r="S99" t="inlineStr">
         <is>
           <t>External</t>
         </is>
       </c>
-      <c r="T98" t="inlineStr"/>
-      <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr">
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr">
         <is>
           <t>PS</t>
         </is>

</xml_diff>